<commit_message>
for newtag and newtag's setup
</commit_message>
<xml_diff>
--- a/lai/valuationquan/HwabaoWPszseinnovation100ETF.xlsx
+++ b/lai/valuationquan/HwabaoWPszseinnovation100ETF.xlsx
@@ -461,10 +461,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U712"/>
+  <dimension ref="A1:U730"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A700" workbookViewId="0">
-      <selection activeCell="A713" sqref="A713"/>
+    <sheetView tabSelected="1" topLeftCell="A713" workbookViewId="0">
+      <selection activeCell="A731" sqref="A731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -33546,23 +33546,23 @@
         <v>0.70500000317891443</v>
       </c>
       <c r="Q527">
-        <f t="shared" ref="Q527:Q712" si="68">SUM(P514:P527)/14</f>
+        <f t="shared" ref="Q527:Q730" si="68">SUM(P514:P527)/14</f>
         <v>0.73757142821947741</v>
       </c>
       <c r="R527">
-        <f t="shared" ref="R527:R712" si="69">P527-Q527</f>
+        <f t="shared" ref="R527:R730" si="69">P527-Q527</f>
         <v>-3.2571425040562985E-2</v>
       </c>
       <c r="S527">
-        <f t="shared" ref="S527:S712" si="70">AVEDEV(P514:P527)</f>
+        <f t="shared" ref="S527:S730" si="70">AVEDEV(P514:P527)</f>
         <v>1.8523810874848144E-2</v>
       </c>
       <c r="T527">
-        <f t="shared" ref="T527:T712" si="71">0.015*S527</f>
+        <f t="shared" ref="T527:T730" si="71">0.015*S527</f>
         <v>2.7785716312272215E-4</v>
       </c>
       <c r="U527">
-        <f t="shared" ref="U527:U712" si="72">R527/T527</f>
+        <f t="shared" ref="U527:U730" si="72">R527/T527</f>
         <v>-117.22362912838439</v>
       </c>
     </row>
@@ -36692,7 +36692,7 @@
         <v>0.65399998426437378</v>
       </c>
       <c r="P577">
-        <f t="shared" ref="P577:P712" si="79">(C577+D577+E577)/3</f>
+        <f t="shared" ref="P577:P730" si="79">(C577+D577+E577)/3</f>
         <v>0.67700000603993737</v>
       </c>
       <c r="Q577">
@@ -36802,7 +36802,7 @@
         <v>42072</v>
       </c>
       <c r="H579">
-        <f t="shared" ref="H579:H712" si="80">H578+1</f>
+        <f t="shared" ref="H579:H730" si="80">H578+1</f>
         <v>577</v>
       </c>
       <c r="I579">
@@ -43992,11 +43992,11 @@
         <v>4510844.3780300291</v>
       </c>
       <c r="N693">
-        <f t="shared" ref="N693:N712" si="91">IF(A693&lt;&gt;$K$37,MAX(N692,VLOOKUP(A693,A:C,3)),)</f>
+        <f t="shared" ref="N693:N711" si="91">IF(A693&lt;&gt;$K$37,MAX(N692,VLOOKUP(A693,A:C,3)),)</f>
         <v>0.68000000715255737</v>
       </c>
       <c r="O693">
-        <f t="shared" ref="O693:O712" si="92">IF(A693&lt;&gt;$K$37,MIN(O692,VLOOKUP(A693,A:D,4)),)</f>
+        <f t="shared" ref="O693:O711" si="92">IF(A693&lt;&gt;$K$37,MIN(O692,VLOOKUP(A693,A:D,4)),)</f>
         <v>0.67000001668930054</v>
       </c>
       <c r="P693">
@@ -45189,12 +45189,12 @@
         <v>4606710.9436179576</v>
       </c>
       <c r="N712">
-        <f t="shared" si="91"/>
-        <v>0</v>
+        <f>VLOOKUP(L38,A:C,3)</f>
+        <v>0.65700000524520874</v>
       </c>
       <c r="O712">
-        <f t="shared" si="92"/>
-        <v>0</v>
+        <f>VLOOKUP(L38,A:D,4)</f>
+        <v>0.64600002765655518</v>
       </c>
       <c r="P712">
         <f t="shared" si="79"/>
@@ -45219,6 +45219,1140 @@
       <c r="U712">
         <f t="shared" si="72"/>
         <v>-76.574709137121957</v>
+      </c>
+    </row>
+    <row r="713" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A713" s="1">
+        <v>45446</v>
+      </c>
+      <c r="B713">
+        <v>0.64800000190734863</v>
+      </c>
+      <c r="C713">
+        <v>0.65700000524520874</v>
+      </c>
+      <c r="D713">
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="E713">
+        <v>0.65399998426437378</v>
+      </c>
+      <c r="F713">
+        <v>8643300</v>
+      </c>
+      <c r="G713">
+        <v>86433</v>
+      </c>
+      <c r="H713">
+        <f t="shared" si="80"/>
+        <v>711</v>
+      </c>
+      <c r="I713">
+        <f>SUM($F$3:F713)/H713</f>
+        <v>4612388.2840629397</v>
+      </c>
+      <c r="N713">
+        <f t="shared" ref="N713:N730" si="93">IF(A713&lt;&gt;$K$38,MAX(N712,VLOOKUP(A713,A:C,3)),)</f>
+        <v>0.65700000524520874</v>
+      </c>
+      <c r="O713">
+        <f t="shared" ref="O713:O730" si="94">IF(A713&lt;&gt;$K$38,MIN(O712,VLOOKUP(A713,A:D,4)),)</f>
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="P713">
+        <f t="shared" si="79"/>
+        <v>0.65233333905537927</v>
+      </c>
+      <c r="Q713">
+        <f t="shared" si="68"/>
+        <v>0.65838095261937102</v>
+      </c>
+      <c r="R713">
+        <f t="shared" si="69"/>
+        <v>-6.0476135639917494E-3</v>
+      </c>
+      <c r="S713">
+        <f t="shared" si="70"/>
+        <v>6.142858948026385E-3</v>
+      </c>
+      <c r="T713">
+        <f t="shared" si="71"/>
+        <v>9.2142884220395768E-5</v>
+      </c>
+      <c r="U713">
+        <f t="shared" si="72"/>
+        <v>-65.632996135941596</v>
+      </c>
+    </row>
+    <row r="714" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A714" s="1">
+        <v>45447</v>
+      </c>
+      <c r="B714">
+        <v>0.65399998426437378</v>
+      </c>
+      <c r="C714">
+        <v>0.66299998760223389</v>
+      </c>
+      <c r="D714">
+        <v>0.65200001001358032</v>
+      </c>
+      <c r="E714">
+        <v>0.66200000047683716</v>
+      </c>
+      <c r="F714">
+        <v>10209700</v>
+      </c>
+      <c r="G714">
+        <v>102097</v>
+      </c>
+      <c r="H714">
+        <f t="shared" si="80"/>
+        <v>712</v>
+      </c>
+      <c r="I714">
+        <f>SUM($F$3:F714)/H714</f>
+        <v>4620249.6769224014</v>
+      </c>
+      <c r="N714">
+        <f t="shared" si="93"/>
+        <v>0.66299998760223389</v>
+      </c>
+      <c r="O714">
+        <f t="shared" si="94"/>
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="P714">
+        <f t="shared" si="79"/>
+        <v>0.65899999936421716</v>
+      </c>
+      <c r="Q714">
+        <f t="shared" si="68"/>
+        <v>0.65807142853736877</v>
+      </c>
+      <c r="R714">
+        <f t="shared" si="69"/>
+        <v>9.2857082684838499E-4</v>
+      </c>
+      <c r="S714">
+        <f t="shared" si="70"/>
+        <v>5.8333348660242045E-3</v>
+      </c>
+      <c r="T714">
+        <f t="shared" si="71"/>
+        <v>8.7500022990363071E-5</v>
+      </c>
+      <c r="U714">
+        <f t="shared" si="72"/>
+        <v>10.61223523279136</v>
+      </c>
+    </row>
+    <row r="715" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A715" s="1">
+        <v>45448</v>
+      </c>
+      <c r="B715">
+        <v>0.66100001335144043</v>
+      </c>
+      <c r="C715">
+        <v>0.66699999570846558</v>
+      </c>
+      <c r="D715">
+        <v>0.6589999794960022</v>
+      </c>
+      <c r="E715">
+        <v>0.6589999794960022</v>
+      </c>
+      <c r="F715">
+        <v>7692509.5</v>
+      </c>
+      <c r="G715">
+        <v>76925.09375</v>
+      </c>
+      <c r="H715">
+        <f t="shared" si="80"/>
+        <v>713</v>
+      </c>
+      <c r="I715">
+        <f>SUM($F$3:F715)/H715</f>
+        <v>4624558.5967303645</v>
+      </c>
+      <c r="N715">
+        <f t="shared" si="93"/>
+        <v>0.66699999570846558</v>
+      </c>
+      <c r="O715">
+        <f t="shared" si="94"/>
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="P715">
+        <f t="shared" si="79"/>
+        <v>0.66166665156682336</v>
+      </c>
+      <c r="Q715">
+        <f t="shared" si="68"/>
+        <v>0.65792857039542429</v>
+      </c>
+      <c r="R715">
+        <f t="shared" si="69"/>
+        <v>3.7380811713990658E-3</v>
+      </c>
+      <c r="S715">
+        <f t="shared" si="70"/>
+        <v>5.690476724079685E-3</v>
+      </c>
+      <c r="T715">
+        <f t="shared" si="71"/>
+        <v>8.535715086119527E-5</v>
+      </c>
+      <c r="U715">
+        <f t="shared" si="72"/>
+        <v>43.793415474677673</v>
+      </c>
+    </row>
+    <row r="716" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A716" s="1">
+        <v>45449</v>
+      </c>
+      <c r="B716">
+        <v>0.6589999794960022</v>
+      </c>
+      <c r="C716">
+        <v>0.66600000858306885</v>
+      </c>
+      <c r="D716">
+        <v>0.65799999237060547</v>
+      </c>
+      <c r="E716">
+        <v>0.65799999237060547</v>
+      </c>
+      <c r="F716">
+        <v>5600600</v>
+      </c>
+      <c r="G716">
+        <v>56006</v>
+      </c>
+      <c r="H716">
+        <f t="shared" si="80"/>
+        <v>714</v>
+      </c>
+      <c r="I716">
+        <f>SUM($F$3:F716)/H716</f>
+        <v>4625925.6014968483</v>
+      </c>
+      <c r="N716">
+        <f t="shared" si="93"/>
+        <v>0.66699999570846558</v>
+      </c>
+      <c r="O716">
+        <f t="shared" si="94"/>
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="P716">
+        <f t="shared" si="79"/>
+        <v>0.66066666444142663</v>
+      </c>
+      <c r="Q716">
+        <f t="shared" si="68"/>
+        <v>0.65771428460166559</v>
+      </c>
+      <c r="R716">
+        <f t="shared" si="69"/>
+        <v>2.9523798397610435E-3</v>
+      </c>
+      <c r="S716">
+        <f t="shared" si="70"/>
+        <v>5.4761909303211133E-3</v>
+      </c>
+      <c r="T716">
+        <f t="shared" si="71"/>
+        <v>8.2142863954816692E-5</v>
+      </c>
+      <c r="U716">
+        <f t="shared" si="72"/>
+        <v>35.942012459962712</v>
+      </c>
+    </row>
+    <row r="717" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A717" s="1">
+        <v>45450</v>
+      </c>
+      <c r="B717">
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="C717">
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="D717">
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="E717">
+        <v>0.64999997615814209</v>
+      </c>
+      <c r="F717">
+        <v>6978200</v>
+      </c>
+      <c r="G717">
+        <v>69782</v>
+      </c>
+      <c r="H717">
+        <f t="shared" si="80"/>
+        <v>715</v>
+      </c>
+      <c r="I717">
+        <f>SUM($F$3:F717)/H717</f>
+        <v>4629215.4957604893</v>
+      </c>
+      <c r="N717">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O717">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P717">
+        <f t="shared" si="79"/>
+        <v>0.65366667509078979</v>
+      </c>
+      <c r="Q717">
+        <f t="shared" si="68"/>
+        <v>0.65669047548657367</v>
+      </c>
+      <c r="R717">
+        <f t="shared" si="69"/>
+        <v>-3.0238003957838711E-3</v>
+      </c>
+      <c r="S717">
+        <f t="shared" si="70"/>
+        <v>4.8843533003411332E-3</v>
+      </c>
+      <c r="T717">
+        <f t="shared" si="71"/>
+        <v>7.3265299505116994E-5</v>
+      </c>
+      <c r="U717">
+        <f t="shared" si="72"/>
+        <v>-41.271931135321203</v>
+      </c>
+    </row>
+    <row r="718" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A718" s="1">
+        <v>45454</v>
+      </c>
+      <c r="B718">
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="C718">
+        <v>0.65100002288818359</v>
+      </c>
+      <c r="D718">
+        <v>0.64300000667572021</v>
+      </c>
+      <c r="E718">
+        <v>0.64999997615814209</v>
+      </c>
+      <c r="F718">
+        <v>7925500</v>
+      </c>
+      <c r="G718">
+        <v>79255</v>
+      </c>
+      <c r="H718">
+        <f t="shared" si="80"/>
+        <v>716</v>
+      </c>
+      <c r="I718">
+        <f>SUM($F$3:F718)/H718</f>
+        <v>4633819.2450680863</v>
+      </c>
+      <c r="N718">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O718">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P718">
+        <f t="shared" si="79"/>
+        <v>0.64800000190734863</v>
+      </c>
+      <c r="Q718">
+        <f t="shared" si="68"/>
+        <v>0.6555476188659668</v>
+      </c>
+      <c r="R718">
+        <f t="shared" si="69"/>
+        <v>-7.5476169586181641E-3</v>
+      </c>
+      <c r="S718">
+        <f t="shared" si="70"/>
+        <v>4.6564624423072508E-3</v>
+      </c>
+      <c r="T718">
+        <f t="shared" si="71"/>
+        <v>6.9846936634608762E-5</v>
+      </c>
+      <c r="U718">
+        <f t="shared" si="72"/>
+        <v>-108.05938416601026</v>
+      </c>
+    </row>
+    <row r="719" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A719" s="1">
+        <v>45455</v>
+      </c>
+      <c r="B719">
+        <v>0.64899998903274536</v>
+      </c>
+      <c r="C719">
+        <v>0.65299999713897705</v>
+      </c>
+      <c r="D719">
+        <v>0.64899998903274536</v>
+      </c>
+      <c r="E719">
+        <v>0.64999997615814209</v>
+      </c>
+      <c r="F719">
+        <v>7330306</v>
+      </c>
+      <c r="G719">
+        <v>73303.0625</v>
+      </c>
+      <c r="H719">
+        <f t="shared" si="80"/>
+        <v>717</v>
+      </c>
+      <c r="I719">
+        <f>SUM($F$3:F719)/H719</f>
+        <v>4637580.0355212688</v>
+      </c>
+      <c r="N719">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O719">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P719">
+        <f t="shared" si="79"/>
+        <v>0.65066665410995483</v>
+      </c>
+      <c r="Q719">
+        <f t="shared" si="68"/>
+        <v>0.65438095018977205</v>
+      </c>
+      <c r="R719">
+        <f t="shared" si="69"/>
+        <v>-3.7142960798172142E-3</v>
+      </c>
+      <c r="S719">
+        <f t="shared" si="70"/>
+        <v>3.7755108609491272E-3</v>
+      </c>
+      <c r="T719">
+        <f t="shared" si="71"/>
+        <v>5.6632662914236907E-5</v>
+      </c>
+      <c r="U719">
+        <f t="shared" si="72"/>
+        <v>-65.585757205908749</v>
+      </c>
+    </row>
+    <row r="720" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A720" s="1">
+        <v>45456</v>
+      </c>
+      <c r="B720">
+        <v>0.65100002288818359</v>
+      </c>
+      <c r="C720">
+        <v>0.65600001811981201</v>
+      </c>
+      <c r="D720">
+        <v>0.64800000190734863</v>
+      </c>
+      <c r="E720">
+        <v>0.64899998903274536</v>
+      </c>
+      <c r="F720">
+        <v>6396090</v>
+      </c>
+      <c r="G720">
+        <v>63960.8984375</v>
+      </c>
+      <c r="H720">
+        <f t="shared" si="80"/>
+        <v>718</v>
+      </c>
+      <c r="I720">
+        <f>SUM($F$3:F720)/H720</f>
+        <v>4640029.2137447773</v>
+      </c>
+      <c r="N720">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O720">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P720">
+        <f t="shared" si="79"/>
+        <v>0.65100000301996863</v>
+      </c>
+      <c r="Q720">
+        <f t="shared" si="68"/>
+        <v>0.65359523608571002</v>
+      </c>
+      <c r="R720">
+        <f t="shared" si="69"/>
+        <v>-2.5952330657413869E-3</v>
+      </c>
+      <c r="S720">
+        <f t="shared" si="70"/>
+        <v>3.1564657379980726E-3</v>
+      </c>
+      <c r="T720">
+        <f t="shared" si="71"/>
+        <v>4.7346986069971089E-5</v>
+      </c>
+      <c r="U720">
+        <f t="shared" si="72"/>
+        <v>-54.813057412061191</v>
+      </c>
+    </row>
+    <row r="721" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A721" s="1">
+        <v>45457</v>
+      </c>
+      <c r="B721">
+        <v>0.6470000147819519</v>
+      </c>
+      <c r="C721">
+        <v>0.65600001811981201</v>
+      </c>
+      <c r="D721">
+        <v>0.64499998092651367</v>
+      </c>
+      <c r="E721">
+        <v>0.65600001811981201</v>
+      </c>
+      <c r="F721">
+        <v>9069805</v>
+      </c>
+      <c r="G721">
+        <v>90698.046875</v>
+      </c>
+      <c r="H721">
+        <f t="shared" si="80"/>
+        <v>719</v>
+      </c>
+      <c r="I721">
+        <f>SUM($F$3:F721)/H721</f>
+        <v>4646190.2370914463</v>
+      </c>
+      <c r="N721">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O721">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P721">
+        <f t="shared" si="79"/>
+        <v>0.65233333905537927</v>
+      </c>
+      <c r="Q721">
+        <f t="shared" si="68"/>
+        <v>0.65340475950922283</v>
+      </c>
+      <c r="R721">
+        <f t="shared" si="69"/>
+        <v>-1.0714204538435634E-3</v>
+      </c>
+      <c r="S721">
+        <f t="shared" si="70"/>
+        <v>3.0918382868474798E-3</v>
+      </c>
+      <c r="T721">
+        <f t="shared" si="71"/>
+        <v>4.6377574302712198E-5</v>
+      </c>
+      <c r="U721">
+        <f t="shared" si="72"/>
+        <v>-23.102123600735752</v>
+      </c>
+    </row>
+    <row r="722" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A722" s="1">
+        <v>45460</v>
+      </c>
+      <c r="B722">
+        <v>0.65200001001358032</v>
+      </c>
+      <c r="C722">
+        <v>0.6600000262260437</v>
+      </c>
+      <c r="D722">
+        <v>0.65200001001358032</v>
+      </c>
+      <c r="E722">
+        <v>0.65799999237060547</v>
+      </c>
+      <c r="F722">
+        <v>7950501</v>
+      </c>
+      <c r="G722">
+        <v>79505.0078125</v>
+      </c>
+      <c r="H722">
+        <f t="shared" si="80"/>
+        <v>720</v>
+      </c>
+      <c r="I722">
+        <f>SUM($F$3:F722)/H722</f>
+        <v>4650779.5575954858</v>
+      </c>
+      <c r="N722">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O722">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P722">
+        <f t="shared" si="79"/>
+        <v>0.65666667620340979</v>
+      </c>
+      <c r="Q722">
+        <f t="shared" si="68"/>
+        <v>0.65361904530298143</v>
+      </c>
+      <c r="R722">
+        <f t="shared" si="69"/>
+        <v>3.0476309004283664E-3</v>
+      </c>
+      <c r="S722">
+        <f t="shared" si="70"/>
+        <v>3.3673485931085068E-3</v>
+      </c>
+      <c r="T722">
+        <f t="shared" si="71"/>
+        <v>5.05102288966276E-5</v>
+      </c>
+      <c r="U722">
+        <f t="shared" si="72"/>
+        <v>60.336905355656519</v>
+      </c>
+    </row>
+    <row r="723" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A723" s="1">
+        <v>45461</v>
+      </c>
+      <c r="B723">
+        <v>0.6600000262260437</v>
+      </c>
+      <c r="C723">
+        <v>0.66299998760223389</v>
+      </c>
+      <c r="D723">
+        <v>0.6589999794960022</v>
+      </c>
+      <c r="E723">
+        <v>0.66100001335144043</v>
+      </c>
+      <c r="F723">
+        <v>9485400</v>
+      </c>
+      <c r="G723">
+        <v>94854</v>
+      </c>
+      <c r="H723">
+        <f t="shared" si="80"/>
+        <v>721</v>
+      </c>
+      <c r="I723">
+        <f>SUM($F$3:F723)/H723</f>
+        <v>4657484.9951022882</v>
+      </c>
+      <c r="N723">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O723">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P723">
+        <f t="shared" si="79"/>
+        <v>0.66099999348322547</v>
+      </c>
+      <c r="Q723">
+        <f t="shared" si="68"/>
+        <v>0.65442856862431475</v>
+      </c>
+      <c r="R723">
+        <f t="shared" si="69"/>
+        <v>6.5714248589107127E-3</v>
+      </c>
+      <c r="S723">
+        <f t="shared" si="70"/>
+        <v>3.8367345625040278E-3</v>
+      </c>
+      <c r="T723">
+        <f t="shared" si="71"/>
+        <v>5.7551018437560416E-5</v>
+      </c>
+      <c r="U723">
+        <f t="shared" si="72"/>
+        <v>114.18433656461414</v>
+      </c>
+    </row>
+    <row r="724" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A724" s="1">
+        <v>45462</v>
+      </c>
+      <c r="B724">
+        <v>0.66299998760223389</v>
+      </c>
+      <c r="C724">
+        <v>0.66299998760223389</v>
+      </c>
+      <c r="D724">
+        <v>0.65600001811981201</v>
+      </c>
+      <c r="E724">
+        <v>0.65700000524520874</v>
+      </c>
+      <c r="F724">
+        <v>5104400</v>
+      </c>
+      <c r="G724">
+        <v>51044</v>
+      </c>
+      <c r="H724">
+        <f t="shared" si="80"/>
+        <v>722</v>
+      </c>
+      <c r="I724">
+        <f>SUM($F$3:F724)/H724</f>
+        <v>4658103.9909539474</v>
+      </c>
+      <c r="N724">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O724">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P724">
+        <f t="shared" si="79"/>
+        <v>0.65866667032241821</v>
+      </c>
+      <c r="Q724">
+        <f t="shared" si="68"/>
+        <v>0.65497618913650524</v>
+      </c>
+      <c r="R724">
+        <f t="shared" si="69"/>
+        <v>3.6904811859129749E-3</v>
+      </c>
+      <c r="S724">
+        <f t="shared" si="70"/>
+        <v>3.9727886517842747E-3</v>
+      </c>
+      <c r="T724">
+        <f t="shared" si="71"/>
+        <v>5.9591829776764117E-5</v>
+      </c>
+      <c r="U724">
+        <f t="shared" si="72"/>
+        <v>61.929314802680501</v>
+      </c>
+    </row>
+    <row r="725" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A725" s="1">
+        <v>45463</v>
+      </c>
+      <c r="B725">
+        <v>0.65399998426437378</v>
+      </c>
+      <c r="C725">
+        <v>0.65399998426437378</v>
+      </c>
+      <c r="D725">
+        <v>0.6470000147819519</v>
+      </c>
+      <c r="E725">
+        <v>0.6470000147819519</v>
+      </c>
+      <c r="F725">
+        <v>6829700</v>
+      </c>
+      <c r="G725">
+        <v>68297</v>
+      </c>
+      <c r="H725">
+        <f t="shared" si="80"/>
+        <v>723</v>
+      </c>
+      <c r="I725">
+        <f>SUM($F$3:F725)/H725</f>
+        <v>4661107.5815612031</v>
+      </c>
+      <c r="N725">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O725">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P725">
+        <f t="shared" si="79"/>
+        <v>0.64933333794275916</v>
+      </c>
+      <c r="Q725">
+        <f t="shared" si="68"/>
+        <v>0.65480952319644747</v>
+      </c>
+      <c r="R725">
+        <f t="shared" si="69"/>
+        <v>-5.4761852536883149E-3</v>
+      </c>
+      <c r="S725">
+        <f t="shared" si="70"/>
+        <v>4.1156451718336916E-3</v>
+      </c>
+      <c r="T725">
+        <f t="shared" si="71"/>
+        <v>6.1734677577505377E-5</v>
+      </c>
+      <c r="U725">
+        <f t="shared" si="72"/>
+        <v>-88.705172985040491</v>
+      </c>
+    </row>
+    <row r="726" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A726" s="1">
+        <v>45464</v>
+      </c>
+      <c r="B726">
+        <v>0.64600002765655518</v>
+      </c>
+      <c r="C726">
+        <v>0.64800000190734863</v>
+      </c>
+      <c r="D726">
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="E726">
+        <v>0.6470000147819519</v>
+      </c>
+      <c r="F726">
+        <v>8226100</v>
+      </c>
+      <c r="G726">
+        <v>82261</v>
+      </c>
+      <c r="H726">
+        <f t="shared" si="80"/>
+        <v>724</v>
+      </c>
+      <c r="I726">
+        <f>SUM($F$3:F726)/H726</f>
+        <v>4666031.6042386051</v>
+      </c>
+      <c r="N726">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O726">
+        <f t="shared" si="94"/>
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="P726">
+        <f t="shared" si="79"/>
+        <v>0.64566667874654138</v>
+      </c>
+      <c r="Q726">
+        <f t="shared" si="68"/>
+        <v>0.65433333459354592</v>
+      </c>
+      <c r="R726">
+        <f t="shared" si="69"/>
+        <v>-8.6666558470045452E-3</v>
+      </c>
+      <c r="S726">
+        <f t="shared" si="70"/>
+        <v>4.5238068314636792E-3</v>
+      </c>
+      <c r="T726">
+        <f t="shared" si="71"/>
+        <v>6.7857102471955181E-5</v>
+      </c>
+      <c r="U726">
+        <f t="shared" si="72"/>
+        <v>-127.71921481006954</v>
+      </c>
+    </row>
+    <row r="727" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A727" s="1">
+        <v>45467</v>
+      </c>
+      <c r="B727">
+        <v>0.64399999380111694</v>
+      </c>
+      <c r="C727">
+        <v>0.6470000147819519</v>
+      </c>
+      <c r="D727">
+        <v>0.63899999856948853</v>
+      </c>
+      <c r="E727">
+        <v>0.63899999856948853</v>
+      </c>
+      <c r="F727">
+        <v>9455300</v>
+      </c>
+      <c r="G727">
+        <v>94553</v>
+      </c>
+      <c r="H727">
+        <f t="shared" si="80"/>
+        <v>725</v>
+      </c>
+      <c r="I727">
+        <f>SUM($F$3:F727)/H727</f>
+        <v>4672637.4916810347</v>
+      </c>
+      <c r="N727">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O727">
+        <f t="shared" si="94"/>
+        <v>0.63899999856948853</v>
+      </c>
+      <c r="P727">
+        <f t="shared" si="79"/>
+        <v>0.64166667064030969</v>
+      </c>
+      <c r="Q727">
+        <f t="shared" si="68"/>
+        <v>0.65357142970675519</v>
+      </c>
+      <c r="R727">
+        <f t="shared" si="69"/>
+        <v>-1.1904759066445503E-2</v>
+      </c>
+      <c r="S727">
+        <f t="shared" si="70"/>
+        <v>5.1904746464320594E-3</v>
+      </c>
+      <c r="T727">
+        <f t="shared" si="71"/>
+        <v>7.7857119696480887E-5</v>
+      </c>
+      <c r="U727">
+        <f t="shared" si="72"/>
+        <v>-152.90520780700797</v>
+      </c>
+    </row>
+    <row r="728" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A728" s="1">
+        <v>45468</v>
+      </c>
+      <c r="B728">
+        <v>0.63499999046325684</v>
+      </c>
+      <c r="C728">
+        <v>0.65100002288818359</v>
+      </c>
+      <c r="D728">
+        <v>0.63200002908706665</v>
+      </c>
+      <c r="E728">
+        <v>0.63400000333786011</v>
+      </c>
+      <c r="F728">
+        <v>7340807</v>
+      </c>
+      <c r="G728">
+        <v>73408.0703125</v>
+      </c>
+      <c r="H728">
+        <f t="shared" si="80"/>
+        <v>726</v>
+      </c>
+      <c r="I728">
+        <f>SUM($F$3:F728)/H728</f>
+        <v>4676312.6562930439</v>
+      </c>
+      <c r="N728">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O728">
+        <f t="shared" si="94"/>
+        <v>0.63200002908706665</v>
+      </c>
+      <c r="P728">
+        <f t="shared" si="79"/>
+        <v>0.63900001843770349</v>
+      </c>
+      <c r="Q728">
+        <f t="shared" si="68"/>
+        <v>0.65214285964057572</v>
+      </c>
+      <c r="R728">
+        <f t="shared" si="69"/>
+        <v>-1.3142841202872235E-2</v>
+      </c>
+      <c r="S728">
+        <f t="shared" si="70"/>
+        <v>5.6666646684919086E-3</v>
+      </c>
+      <c r="T728">
+        <f t="shared" si="71"/>
+        <v>8.499997002737863E-5</v>
+      </c>
+      <c r="U728">
+        <f t="shared" si="72"/>
+        <v>-154.62171573282797</v>
+      </c>
+    </row>
+    <row r="729" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A729" s="1">
+        <v>45469</v>
+      </c>
+      <c r="B729">
+        <v>0.63499999046325684</v>
+      </c>
+      <c r="C729">
+        <v>0.64300000667572021</v>
+      </c>
+      <c r="D729">
+        <v>0.63300001621246338</v>
+      </c>
+      <c r="E729">
+        <v>0.64200001955032349</v>
+      </c>
+      <c r="F729">
+        <v>3352000</v>
+      </c>
+      <c r="G729">
+        <v>33520</v>
+      </c>
+      <c r="H729">
+        <f t="shared" si="80"/>
+        <v>727</v>
+      </c>
+      <c r="I729">
+        <f>SUM($F$3:F729)/H729</f>
+        <v>4674491.0432857638</v>
+      </c>
+      <c r="N729">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O729">
+        <f t="shared" si="94"/>
+        <v>0.63200002908706665</v>
+      </c>
+      <c r="P729">
+        <f t="shared" si="79"/>
+        <v>0.63933334747950232</v>
+      </c>
+      <c r="Q729">
+        <f t="shared" si="68"/>
+        <v>0.65054762363433838</v>
+      </c>
+      <c r="R729">
+        <f t="shared" si="69"/>
+        <v>-1.1214276154836056E-2</v>
+      </c>
+      <c r="S729">
+        <f t="shared" si="70"/>
+        <v>5.7550980931236574E-3</v>
+      </c>
+      <c r="T729">
+        <f t="shared" si="71"/>
+        <v>8.632647139685486E-5</v>
+      </c>
+      <c r="U729">
+        <f t="shared" si="72"/>
+        <v>-129.90541572448225</v>
+      </c>
+    </row>
+    <row r="730" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A730" s="1">
+        <v>45470</v>
+      </c>
+      <c r="B730">
+        <v>0.63899999856948853</v>
+      </c>
+      <c r="C730">
+        <v>0.63999998569488525</v>
+      </c>
+      <c r="D730">
+        <v>0.63499999046325684</v>
+      </c>
+      <c r="E730">
+        <v>0.63499999046325684</v>
+      </c>
+      <c r="F730">
+        <v>8155900</v>
+      </c>
+      <c r="G730">
+        <v>81559</v>
+      </c>
+      <c r="H730">
+        <f t="shared" si="80"/>
+        <v>728</v>
+      </c>
+      <c r="I730">
+        <f>SUM($F$3:F730)/H730</f>
+        <v>4679273.1984460847</v>
+      </c>
+      <c r="N730">
+        <f t="shared" si="93"/>
+        <v>0.66900002956390381</v>
+      </c>
+      <c r="O730">
+        <f t="shared" si="94"/>
+        <v>0.63200002908706665</v>
+      </c>
+      <c r="P730">
+        <f t="shared" si="79"/>
+        <v>0.63666665554046631</v>
+      </c>
+      <c r="Q730">
+        <f t="shared" si="68"/>
+        <v>0.64883333728426973</v>
+      </c>
+      <c r="R730">
+        <f t="shared" si="69"/>
+        <v>-1.216668174380342E-2</v>
+      </c>
+      <c r="S730">
+        <f t="shared" si="70"/>
+        <v>6.0952358505352777E-3</v>
+      </c>
+      <c r="T730">
+        <f t="shared" si="71"/>
+        <v>9.1428537758029166E-5</v>
+      </c>
+      <c r="U730">
+        <f t="shared" si="72"/>
+        <v>-133.07313057989876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>